<commit_message>
marked things with completed
</commit_message>
<xml_diff>
--- a/etc/merfoldko_01_elem_lista.xlsx
+++ b/etc/merfoldko_01_elem_lista.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csiko\Documents\Coding\Webterv-1\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC8952A-9538-4BD1-8762-B7D4BC03A95E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A894A902-6013-4336-963E-CA35DE3A0ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="88">
   <si>
     <t>2. Általános szempontok (max. 45 pont)</t>
   </si>
@@ -299,6 +299,9 @@
   </si>
   <si>
     <t>2</t>
+  </si>
+  <si>
+    <t>1 személyre</t>
   </si>
 </sst>
 </file>
@@ -408,7 +411,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -431,22 +434,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -514,10 +506,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -526,6 +514,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -857,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,10 +867,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="29"/>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
@@ -888,10 +883,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="28"/>
+      <c r="C5" s="26"/>
     </row>
     <row r="6" spans="1:8" s="3" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
@@ -950,7 +945,7 @@
       </c>
       <c r="E9" s="23"/>
       <c r="F9" s="24"/>
-      <c r="G9" s="27" t="str">
+      <c r="G9" s="25" t="str">
         <f>IF(E9*B9=0,"",E9*B9)</f>
         <v/>
       </c>
@@ -967,7 +962,7 @@
       </c>
       <c r="E10" s="23"/>
       <c r="F10" s="24"/>
-      <c r="G10" s="27" t="str">
+      <c r="G10" s="25" t="str">
         <f t="shared" ref="G10:G65" si="0">IF(E10*B10=0,"",E10*B10)</f>
         <v/>
       </c>
@@ -984,7 +979,7 @@
       </c>
       <c r="E11" s="23"/>
       <c r="F11" s="24"/>
-      <c r="G11" s="27" t="str">
+      <c r="G11" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1001,7 +996,7 @@
       </c>
       <c r="E12" s="23"/>
       <c r="F12" s="24"/>
-      <c r="G12" s="27" t="str">
+      <c r="G12" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1018,7 +1013,7 @@
       </c>
       <c r="E13" s="23"/>
       <c r="F13" s="24"/>
-      <c r="G13" s="27" t="str">
+      <c r="G13" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1043,7 +1038,7 @@
       <c r="F14" s="23">
         <v>1</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G14" s="25">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1060,7 +1055,7 @@
       </c>
       <c r="E15" s="23"/>
       <c r="F15" s="24"/>
-      <c r="G15" s="27" t="str">
+      <c r="G15" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1075,7 +1070,7 @@
       <c r="D16" s="7"/>
       <c r="E16" s="10"/>
       <c r="F16" s="7"/>
-      <c r="G16" s="27" t="str">
+      <c r="G16" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1097,8 +1092,8 @@
       <c r="F17" s="23">
         <v>1</v>
       </c>
-      <c r="G17" s="27">
-        <f t="shared" si="0"/>
+      <c r="G17" s="25">
+        <f>IF(E17*B17=0,"",E17*B17)</f>
         <v>2</v>
       </c>
       <c r="H17" s="19" t="s">
@@ -1114,9 +1109,8 @@
       </c>
       <c r="E18" s="23"/>
       <c r="F18" s="24"/>
-      <c r="G18" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="G18" s="25">
+        <v>2</v>
       </c>
       <c r="H18" s="19" t="s">
         <v>12</v>
@@ -1131,9 +1125,8 @@
       </c>
       <c r="E19" s="23"/>
       <c r="F19" s="24"/>
-      <c r="G19" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="G19" s="25">
+        <v>2</v>
       </c>
       <c r="H19" s="19" t="s">
         <v>13</v>
@@ -1152,7 +1145,7 @@
       <c r="F20" s="23">
         <v>1</v>
       </c>
-      <c r="G20" s="27" t="str">
+      <c r="G20" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1167,7 +1160,7 @@
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
-      <c r="G21" s="27" t="str">
+      <c r="G21" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1183,7 +1176,7 @@
         <v>6</v>
       </c>
       <c r="F22" s="24"/>
-      <c r="G22" s="27" t="str">
+      <c r="G22" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1204,7 +1197,7 @@
       <c r="F23" s="23">
         <v>2</v>
       </c>
-      <c r="G23" s="27" t="str">
+      <c r="G23" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1221,7 +1214,7 @@
       </c>
       <c r="E24" s="23"/>
       <c r="F24" s="24"/>
-      <c r="G24" s="27" t="str">
+      <c r="G24" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1236,7 +1229,7 @@
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
-      <c r="G25" s="27" t="str">
+      <c r="G25" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1254,7 +1247,7 @@
       <c r="F26" s="23">
         <v>2</v>
       </c>
-      <c r="G26" s="27" t="str">
+      <c r="G26" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1271,7 +1264,7 @@
       <c r="D27" s="13"/>
       <c r="E27" s="13"/>
       <c r="F27" s="11"/>
-      <c r="G27" s="27" t="str">
+      <c r="G27" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1282,7 +1275,7 @@
         <v>69</v>
       </c>
       <c r="F28" s="7"/>
-      <c r="G28" s="27" t="str">
+      <c r="G28" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1304,7 +1297,7 @@
       <c r="F29" s="20">
         <v>1</v>
       </c>
-      <c r="G29" s="27">
+      <c r="G29" s="25">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -1329,7 +1322,7 @@
       <c r="F30" s="20">
         <v>1</v>
       </c>
-      <c r="G30" s="27">
+      <c r="G30" s="25">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -1354,7 +1347,7 @@
       <c r="F31" s="20">
         <v>1</v>
       </c>
-      <c r="G31" s="27">
+      <c r="G31" s="25">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -1379,7 +1372,7 @@
       <c r="F32" s="20">
         <v>1</v>
       </c>
-      <c r="G32" s="27">
+      <c r="G32" s="25">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -1404,7 +1397,7 @@
       <c r="F33" s="20">
         <v>1</v>
       </c>
-      <c r="G33" s="27">
+      <c r="G33" s="25">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -1417,7 +1410,7 @@
         <v>70</v>
       </c>
       <c r="E34" s="1"/>
-      <c r="G34" s="27" t="str">
+      <c r="G34" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1439,7 +1432,7 @@
       <c r="F35" s="20">
         <v>3</v>
       </c>
-      <c r="G35" s="27">
+      <c r="G35" s="25">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -1452,7 +1445,7 @@
         <v>72</v>
       </c>
       <c r="E36" s="1"/>
-      <c r="G36" s="27" t="str">
+      <c r="G36" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1470,7 +1463,7 @@
       <c r="F37" s="20">
         <v>1</v>
       </c>
-      <c r="G37" s="27" t="str">
+      <c r="G37" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1491,7 +1484,7 @@
       <c r="F38" s="20">
         <v>1</v>
       </c>
-      <c r="G38" s="27" t="str">
+      <c r="G38" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1512,7 +1505,7 @@
       <c r="F39" s="20">
         <v>1</v>
       </c>
-      <c r="G39" s="27" t="str">
+      <c r="G39" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1524,7 +1517,7 @@
       <c r="A40" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="G40" s="27" t="str">
+      <c r="G40" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1546,7 +1539,7 @@
       <c r="F41" s="20">
         <v>1</v>
       </c>
-      <c r="G41" s="27">
+      <c r="G41" s="25">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1571,7 +1564,7 @@
       <c r="F42" s="20">
         <v>1</v>
       </c>
-      <c r="G42" s="27">
+      <c r="G42" s="25">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1596,7 +1589,7 @@
       <c r="F43" s="20">
         <v>1</v>
       </c>
-      <c r="G43" s="27">
+      <c r="G43" s="25">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1621,7 +1614,7 @@
       <c r="F44" s="20">
         <v>1</v>
       </c>
-      <c r="G44" s="27">
+      <c r="G44" s="25">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1646,7 +1639,7 @@
       <c r="F45" s="20">
         <v>1</v>
       </c>
-      <c r="G45" s="27">
+      <c r="G45" s="25">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1671,7 +1664,7 @@
       <c r="F46" s="20">
         <v>1</v>
       </c>
-      <c r="G46" s="27">
+      <c r="G46" s="25">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1696,7 +1689,7 @@
       <c r="F47" s="20">
         <v>1</v>
       </c>
-      <c r="G47" s="27">
+      <c r="G47" s="25">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1721,7 +1714,7 @@
       <c r="F48" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="G48" s="27">
+      <c r="G48" s="25">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -1746,7 +1739,7 @@
       <c r="F49" s="20">
         <v>2</v>
       </c>
-      <c r="G49" s="27">
+      <c r="G49" s="25">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -1767,7 +1760,7 @@
       <c r="F50" s="20">
         <v>1</v>
       </c>
-      <c r="G50" s="27" t="str">
+      <c r="G50" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1786,7 +1779,7 @@
         <v>3</v>
       </c>
       <c r="F51" s="22"/>
-      <c r="G51" s="27" t="str">
+      <c r="G51" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1798,7 +1791,7 @@
       <c r="A52" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="G52" s="27" t="str">
+      <c r="G52" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1820,7 +1813,7 @@
       <c r="F53" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="G53" s="27">
+      <c r="G53" s="25">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1832,7 +1825,7 @@
       <c r="A54" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="G54" s="27" t="str">
+      <c r="G54" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1854,7 +1847,7 @@
       <c r="F55" s="20">
         <v>4</v>
       </c>
-      <c r="G55" s="27">
+      <c r="G55" s="25">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -1879,7 +1872,7 @@
       <c r="F56" s="20">
         <v>1</v>
       </c>
-      <c r="G56" s="27">
+      <c r="G56" s="25">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1904,7 +1897,7 @@
       <c r="F57" s="20">
         <v>1</v>
       </c>
-      <c r="G57" s="27">
+      <c r="G57" s="25">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -1916,7 +1909,7 @@
       <c r="A58" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="G58" s="27" t="str">
+      <c r="G58" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1938,7 +1931,7 @@
       <c r="F59" s="20">
         <v>1</v>
       </c>
-      <c r="G59" s="27">
+      <c r="G59" s="25">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1963,7 +1956,7 @@
       <c r="F60" s="20">
         <v>1</v>
       </c>
-      <c r="G60" s="27">
+      <c r="G60" s="25">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1988,7 +1981,7 @@
       <c r="F61" s="20">
         <v>1</v>
       </c>
-      <c r="G61" s="27">
+      <c r="G61" s="25">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2013,7 +2006,7 @@
       <c r="F62" s="20">
         <v>1</v>
       </c>
-      <c r="G62" s="27">
+      <c r="G62" s="25">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2038,7 +2031,7 @@
       <c r="F63" s="20">
         <v>3</v>
       </c>
-      <c r="G63" s="27">
+      <c r="G63" s="25">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -2063,7 +2056,7 @@
       <c r="F64" s="20">
         <v>1</v>
       </c>
-      <c r="G64" s="27">
+      <c r="G64" s="25">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2084,7 +2077,7 @@
       <c r="F65" s="20">
         <v>2</v>
       </c>
-      <c r="G65" s="27" t="str">
+      <c r="G65" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -2093,12 +2086,19 @@
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F68" s="25" t="s">
+      <c r="D68" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="G68" s="26">
+      <c r="E68" s="29">
         <f>SUM(G9:G65)</f>
-        <v>44</v>
+        <v>48</v>
+      </c>
+      <c r="F68" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="G68" s="30">
+        <f>E68/2</f>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>